<commit_message>
Versione definitiva della tesi, versione stampata per segreteria.
</commit_message>
<xml_diff>
--- a/Dataset/DatasetDefinitivo/DatesetConfronto.xlsx
+++ b/Dataset/DatasetDefinitivo/DatesetConfronto.xlsx
@@ -956,12 +956,6 @@
     <t>Concordi</t>
   </si>
   <si>
-    <t>Agreement polaritá</t>
-  </si>
-  <si>
-    <t>Agreement emozione</t>
-  </si>
-  <si>
     <t>Media totale emozioni</t>
   </si>
   <si>
@@ -973,6 +967,12 @@
     <t>Su 268 frasi solo su 15 c'è unanimitá sulle emozioni
 tra le tre persone che hanno fornito
 i tag</t>
+  </si>
+  <si>
+    <t>Intesa polaritá</t>
+  </si>
+  <si>
+    <t>Intesa emozioni</t>
   </si>
 </sst>
 </file>
@@ -1526,33 +1526,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1570,15 +1547,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1622,31 +1590,43 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2016,16 +1996,16 @@
       <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="93"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:21" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -11691,15 +11671,15 @@
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B270">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B270">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Falso">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Falso">
       <formula>NOT(ISERROR(SEARCH("Falso",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11736,7 +11716,7 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="127" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="115" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="14" style="5" customWidth="1"/>
@@ -11744,7 +11724,7 @@
     <col min="7" max="7" width="9.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="128" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="116" customWidth="1"/>
     <col min="11" max="11" width="24.140625" style="5" customWidth="1"/>
     <col min="12" max="12" width="25" style="5" customWidth="1"/>
     <col min="13" max="13" width="17.140625" style="6" customWidth="1"/>
@@ -11761,63 +11741,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="109" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="110" t="s">
+      <c r="A1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="112"/>
-    </row>
-    <row r="2" spans="1:21" s="115" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="113"/>
-      <c r="B2" s="109" t="s">
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="122"/>
+    </row>
+    <row r="2" spans="1:21" s="103" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="101"/>
+      <c r="B2" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="113" t="s">
+      <c r="C2" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="113" t="s">
+      <c r="G2" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="113" t="s">
+      <c r="H2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="113" t="s">
+      <c r="I2" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="114" t="s">
+      <c r="J2" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
     </row>
     <row r="3" spans="1:21" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -11847,20 +11827,20 @@
       <c r="I3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="116" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
+      <c r="J3" s="104" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
     </row>
     <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -16806,19 +16786,19 @@
       <c r="E158" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F158" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="G158" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="H158" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="I158" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="J158" s="119" t="s">
+      <c r="F158" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G158" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="H158" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I158" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="J158" s="107" t="s">
         <v>14</v>
       </c>
     </row>
@@ -16826,31 +16806,31 @@
       <c r="A159" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B159" s="120">
+      <c r="B159" s="108">
         <v>3</v>
       </c>
-      <c r="C159" s="121" t="s">
-        <v>13</v>
-      </c>
-      <c r="D159" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="E159" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="F159" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="G159" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="H159" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="I159" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="J159" s="123" t="s">
+      <c r="C159" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D159" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="G159" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="H159" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="I159" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="J159" s="111" t="s">
         <v>14</v>
       </c>
     </row>
@@ -16858,31 +16838,31 @@
       <c r="A160" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B160" s="120">
+      <c r="B160" s="108">
         <v>3</v>
       </c>
-      <c r="C160" s="121" t="s">
-        <v>13</v>
-      </c>
-      <c r="D160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="E160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="F160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="G160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="H160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="I160" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="J160" s="123" t="s">
+      <c r="C160" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="G160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="H160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="J160" s="111" t="s">
         <v>13</v>
       </c>
     </row>
@@ -16893,10 +16873,10 @@
       <c r="B161" s="77">
         <v>2</v>
       </c>
-      <c r="C161" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D161" s="118" t="s">
+      <c r="C161" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D161" s="106" t="s">
         <v>13</v>
       </c>
       <c r="E161" s="6" t="s">
@@ -18830,22 +18810,22 @@
       <c r="D221" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E221" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="F221" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="G221" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="H221" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="I221" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="J221" s="123" t="s">
+      <c r="E221" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F221" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="G221" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="H221" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="I221" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="J221" s="111" t="s">
         <v>14</v>
       </c>
     </row>
@@ -18856,28 +18836,28 @@
       <c r="B222" s="8">
         <v>3</v>
       </c>
-      <c r="C222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="E222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="F222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="G222" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="H222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="I222" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="J222" s="119" t="s">
+      <c r="C222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="E222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G222" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="H222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I222" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="J222" s="107" t="s">
         <v>14</v>
       </c>
     </row>
@@ -19194,10 +19174,10 @@
       <c r="H232" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I232" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="J232" s="119" t="s">
+      <c r="I232" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="J232" s="107" t="s">
         <v>13</v>
       </c>
     </row>
@@ -19208,28 +19188,28 @@
       <c r="B233" s="77">
         <v>4</v>
       </c>
-      <c r="C233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="E233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="F233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="G233" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="H233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="I233" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="J233" s="119" t="s">
+      <c r="C233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="E233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G233" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="H233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I233" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="J233" s="107" t="s">
         <v>13</v>
       </c>
     </row>
@@ -19240,28 +19220,28 @@
       <c r="B234" s="77">
         <v>4</v>
       </c>
-      <c r="C234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="E234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="F234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="G234" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="H234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="I234" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="J234" s="119" t="s">
+      <c r="C234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="E234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G234" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="H234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I234" s="106" t="s">
+        <v>13</v>
+      </c>
+      <c r="J234" s="107" t="s">
         <v>14</v>
       </c>
     </row>
@@ -20418,188 +20398,188 @@
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A272" s="124"/>
-      <c r="B272" s="125"/>
-      <c r="C272" s="124"/>
-      <c r="D272" s="124"/>
-      <c r="E272" s="124"/>
-      <c r="F272" s="124"/>
-      <c r="G272" s="124"/>
-      <c r="H272" s="124"/>
-      <c r="I272" s="124"/>
-      <c r="J272" s="126"/>
-      <c r="K272" s="124"/>
-      <c r="L272" s="124"/>
-      <c r="M272" s="124"/>
-      <c r="N272" s="124"/>
-      <c r="O272" s="124"/>
-      <c r="P272" s="124"/>
-      <c r="Q272" s="124"/>
-      <c r="R272" s="124"/>
-      <c r="S272" s="124"/>
-      <c r="T272" s="124"/>
-      <c r="U272" s="124"/>
+      <c r="A272" s="112"/>
+      <c r="B272" s="113"/>
+      <c r="C272" s="112"/>
+      <c r="D272" s="112"/>
+      <c r="E272" s="112"/>
+      <c r="F272" s="112"/>
+      <c r="G272" s="112"/>
+      <c r="H272" s="112"/>
+      <c r="I272" s="112"/>
+      <c r="J272" s="114"/>
+      <c r="K272" s="112"/>
+      <c r="L272" s="112"/>
+      <c r="M272" s="112"/>
+      <c r="N272" s="112"/>
+      <c r="O272" s="112"/>
+      <c r="P272" s="112"/>
+      <c r="Q272" s="112"/>
+      <c r="R272" s="112"/>
+      <c r="S272" s="112"/>
+      <c r="T272" s="112"/>
+      <c r="U272" s="112"/>
     </row>
     <row r="273" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A273" s="124"/>
-      <c r="B273" s="125"/>
-      <c r="C273" s="124"/>
-      <c r="D273" s="124"/>
-      <c r="E273" s="124"/>
-      <c r="F273" s="124"/>
-      <c r="G273" s="124"/>
-      <c r="H273" s="124"/>
-      <c r="I273" s="124"/>
-      <c r="J273" s="126"/>
-      <c r="K273" s="124"/>
-      <c r="L273" s="124"/>
-      <c r="M273" s="124"/>
-      <c r="N273" s="124"/>
-      <c r="O273" s="124"/>
-      <c r="P273" s="124"/>
-      <c r="Q273" s="124"/>
-      <c r="R273" s="124"/>
-      <c r="S273" s="124"/>
-      <c r="T273" s="124"/>
-      <c r="U273" s="124"/>
+      <c r="A273" s="112"/>
+      <c r="B273" s="113"/>
+      <c r="C273" s="112"/>
+      <c r="D273" s="112"/>
+      <c r="E273" s="112"/>
+      <c r="F273" s="112"/>
+      <c r="G273" s="112"/>
+      <c r="H273" s="112"/>
+      <c r="I273" s="112"/>
+      <c r="J273" s="114"/>
+      <c r="K273" s="112"/>
+      <c r="L273" s="112"/>
+      <c r="M273" s="112"/>
+      <c r="N273" s="112"/>
+      <c r="O273" s="112"/>
+      <c r="P273" s="112"/>
+      <c r="Q273" s="112"/>
+      <c r="R273" s="112"/>
+      <c r="S273" s="112"/>
+      <c r="T273" s="112"/>
+      <c r="U273" s="112"/>
     </row>
     <row r="274" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A274" s="124"/>
-      <c r="B274" s="125"/>
-      <c r="C274" s="124"/>
-      <c r="D274" s="124"/>
-      <c r="E274" s="124"/>
-      <c r="F274" s="124"/>
-      <c r="G274" s="124"/>
-      <c r="H274" s="124"/>
-      <c r="I274" s="124"/>
-      <c r="J274" s="126"/>
-      <c r="K274" s="124"/>
-      <c r="L274" s="124"/>
-      <c r="M274" s="124"/>
-      <c r="N274" s="124"/>
-      <c r="O274" s="124"/>
-      <c r="P274" s="124"/>
-      <c r="Q274" s="124"/>
-      <c r="R274" s="124"/>
-      <c r="S274" s="124"/>
-      <c r="T274" s="124"/>
-      <c r="U274" s="124"/>
+      <c r="A274" s="112"/>
+      <c r="B274" s="113"/>
+      <c r="C274" s="112"/>
+      <c r="D274" s="112"/>
+      <c r="E274" s="112"/>
+      <c r="F274" s="112"/>
+      <c r="G274" s="112"/>
+      <c r="H274" s="112"/>
+      <c r="I274" s="112"/>
+      <c r="J274" s="114"/>
+      <c r="K274" s="112"/>
+      <c r="L274" s="112"/>
+      <c r="M274" s="112"/>
+      <c r="N274" s="112"/>
+      <c r="O274" s="112"/>
+      <c r="P274" s="112"/>
+      <c r="Q274" s="112"/>
+      <c r="R274" s="112"/>
+      <c r="S274" s="112"/>
+      <c r="T274" s="112"/>
+      <c r="U274" s="112"/>
     </row>
     <row r="275" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A275" s="124"/>
-      <c r="B275" s="125"/>
-      <c r="C275" s="124"/>
-      <c r="D275" s="124"/>
-      <c r="E275" s="124"/>
-      <c r="F275" s="124"/>
-      <c r="G275" s="124"/>
-      <c r="H275" s="124"/>
-      <c r="I275" s="124"/>
-      <c r="J275" s="126"/>
-      <c r="K275" s="124"/>
-      <c r="L275" s="124"/>
-      <c r="M275" s="124"/>
-      <c r="N275" s="124"/>
-      <c r="O275" s="124"/>
-      <c r="P275" s="124"/>
-      <c r="Q275" s="124"/>
-      <c r="R275" s="124"/>
-      <c r="S275" s="124"/>
-      <c r="T275" s="124"/>
-      <c r="U275" s="124"/>
+      <c r="A275" s="112"/>
+      <c r="B275" s="113"/>
+      <c r="C275" s="112"/>
+      <c r="D275" s="112"/>
+      <c r="E275" s="112"/>
+      <c r="F275" s="112"/>
+      <c r="G275" s="112"/>
+      <c r="H275" s="112"/>
+      <c r="I275" s="112"/>
+      <c r="J275" s="114"/>
+      <c r="K275" s="112"/>
+      <c r="L275" s="112"/>
+      <c r="M275" s="112"/>
+      <c r="N275" s="112"/>
+      <c r="O275" s="112"/>
+      <c r="P275" s="112"/>
+      <c r="Q275" s="112"/>
+      <c r="R275" s="112"/>
+      <c r="S275" s="112"/>
+      <c r="T275" s="112"/>
+      <c r="U275" s="112"/>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A276" s="124"/>
-      <c r="B276" s="125"/>
-      <c r="C276" s="124"/>
-      <c r="D276" s="124"/>
-      <c r="E276" s="124"/>
-      <c r="F276" s="124"/>
-      <c r="G276" s="124"/>
-      <c r="H276" s="124"/>
-      <c r="I276" s="124"/>
-      <c r="J276" s="126"/>
-      <c r="K276" s="124"/>
-      <c r="L276" s="124"/>
-      <c r="M276" s="124"/>
-      <c r="N276" s="124"/>
-      <c r="O276" s="124"/>
-      <c r="P276" s="124"/>
-      <c r="Q276" s="124"/>
-      <c r="R276" s="124"/>
-      <c r="S276" s="124"/>
-      <c r="T276" s="124"/>
-      <c r="U276" s="124"/>
+      <c r="A276" s="112"/>
+      <c r="B276" s="113"/>
+      <c r="C276" s="112"/>
+      <c r="D276" s="112"/>
+      <c r="E276" s="112"/>
+      <c r="F276" s="112"/>
+      <c r="G276" s="112"/>
+      <c r="H276" s="112"/>
+      <c r="I276" s="112"/>
+      <c r="J276" s="114"/>
+      <c r="K276" s="112"/>
+      <c r="L276" s="112"/>
+      <c r="M276" s="112"/>
+      <c r="N276" s="112"/>
+      <c r="O276" s="112"/>
+      <c r="P276" s="112"/>
+      <c r="Q276" s="112"/>
+      <c r="R276" s="112"/>
+      <c r="S276" s="112"/>
+      <c r="T276" s="112"/>
+      <c r="U276" s="112"/>
     </row>
     <row r="277" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A277" s="124"/>
-      <c r="B277" s="125"/>
-      <c r="C277" s="124"/>
-      <c r="D277" s="124"/>
-      <c r="E277" s="124"/>
-      <c r="F277" s="124"/>
-      <c r="G277" s="124"/>
-      <c r="H277" s="124"/>
-      <c r="I277" s="124"/>
-      <c r="J277" s="126"/>
-      <c r="K277" s="124"/>
-      <c r="L277" s="124"/>
-      <c r="M277" s="124"/>
-      <c r="N277" s="124"/>
-      <c r="O277" s="124"/>
-      <c r="P277" s="124"/>
-      <c r="Q277" s="124"/>
-      <c r="R277" s="124"/>
-      <c r="S277" s="124"/>
-      <c r="T277" s="124"/>
-      <c r="U277" s="124"/>
+      <c r="A277" s="112"/>
+      <c r="B277" s="113"/>
+      <c r="C277" s="112"/>
+      <c r="D277" s="112"/>
+      <c r="E277" s="112"/>
+      <c r="F277" s="112"/>
+      <c r="G277" s="112"/>
+      <c r="H277" s="112"/>
+      <c r="I277" s="112"/>
+      <c r="J277" s="114"/>
+      <c r="K277" s="112"/>
+      <c r="L277" s="112"/>
+      <c r="M277" s="112"/>
+      <c r="N277" s="112"/>
+      <c r="O277" s="112"/>
+      <c r="P277" s="112"/>
+      <c r="Q277" s="112"/>
+      <c r="R277" s="112"/>
+      <c r="S277" s="112"/>
+      <c r="T277" s="112"/>
+      <c r="U277" s="112"/>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A278" s="124"/>
-      <c r="B278" s="125"/>
-      <c r="C278" s="124"/>
-      <c r="D278" s="124"/>
-      <c r="E278" s="124"/>
-      <c r="F278" s="124"/>
-      <c r="G278" s="124"/>
-      <c r="H278" s="124"/>
-      <c r="I278" s="124"/>
-      <c r="J278" s="126"/>
-      <c r="K278" s="124"/>
-      <c r="L278" s="124"/>
-      <c r="M278" s="124"/>
-      <c r="N278" s="124"/>
-      <c r="O278" s="124"/>
-      <c r="P278" s="124"/>
-      <c r="Q278" s="124"/>
-      <c r="R278" s="124"/>
-      <c r="S278" s="124"/>
-      <c r="T278" s="124"/>
-      <c r="U278" s="124"/>
+      <c r="A278" s="112"/>
+      <c r="B278" s="113"/>
+      <c r="C278" s="112"/>
+      <c r="D278" s="112"/>
+      <c r="E278" s="112"/>
+      <c r="F278" s="112"/>
+      <c r="G278" s="112"/>
+      <c r="H278" s="112"/>
+      <c r="I278" s="112"/>
+      <c r="J278" s="114"/>
+      <c r="K278" s="112"/>
+      <c r="L278" s="112"/>
+      <c r="M278" s="112"/>
+      <c r="N278" s="112"/>
+      <c r="O278" s="112"/>
+      <c r="P278" s="112"/>
+      <c r="Q278" s="112"/>
+      <c r="R278" s="112"/>
+      <c r="S278" s="112"/>
+      <c r="T278" s="112"/>
+      <c r="U278" s="112"/>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A279" s="124"/>
-      <c r="B279" s="125"/>
-      <c r="C279" s="124"/>
-      <c r="D279" s="124"/>
-      <c r="E279" s="124"/>
-      <c r="F279" s="124"/>
-      <c r="G279" s="124"/>
-      <c r="H279" s="124"/>
-      <c r="I279" s="124"/>
-      <c r="J279" s="126"/>
-      <c r="K279" s="124"/>
-      <c r="L279" s="124"/>
-      <c r="M279" s="124"/>
-      <c r="N279" s="124"/>
-      <c r="O279" s="124"/>
-      <c r="P279" s="124"/>
-      <c r="Q279" s="124"/>
-      <c r="R279" s="124"/>
-      <c r="S279" s="124"/>
-      <c r="T279" s="124"/>
-      <c r="U279" s="124"/>
+      <c r="A279" s="112"/>
+      <c r="B279" s="113"/>
+      <c r="C279" s="112"/>
+      <c r="D279" s="112"/>
+      <c r="E279" s="112"/>
+      <c r="F279" s="112"/>
+      <c r="G279" s="112"/>
+      <c r="H279" s="112"/>
+      <c r="I279" s="112"/>
+      <c r="J279" s="114"/>
+      <c r="K279" s="112"/>
+      <c r="L279" s="112"/>
+      <c r="M279" s="112"/>
+      <c r="N279" s="112"/>
+      <c r="O279" s="112"/>
+      <c r="P279" s="112"/>
+      <c r="Q279" s="112"/>
+      <c r="R279" s="112"/>
+      <c r="S279" s="112"/>
+      <c r="T279" s="112"/>
+      <c r="U279" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -20669,16 +20649,16 @@
       <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="96"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="125"/>
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
       <c r="M1" s="44"/>
@@ -53945,16 +53925,16 @@
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="93"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="119"/>
       <c r="K1" s="87"/>
       <c r="L1" s="87"/>
     </row>
@@ -68098,7 +68078,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68112,26 +68092,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="103"/>
+      <c r="B1" s="94"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="104" t="s">
-        <v>291</v>
-      </c>
-      <c r="C2" s="101" t="s">
-        <v>292</v>
-      </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
+      <c r="B2" s="95" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="126" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="128"/>
       <c r="K2" s="39"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="103"/>
+      <c r="B3" s="94"/>
       <c r="C3" s="36" t="s">
         <v>4</v>
       </c>
@@ -68153,7 +68133,7 @@
       <c r="I3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="99" t="s">
+      <c r="J3" s="91" t="s">
         <v>11</v>
       </c>
     </row>
@@ -68161,7 +68141,7 @@
       <c r="A4" t="s">
         <v>290</v>
       </c>
-      <c r="B4" s="105">
+      <c r="B4" s="96">
         <f>SUM(Confronto!B3:B270)</f>
         <v>174</v>
       </c>
@@ -68203,7 +68183,7 @@
       <c r="A5" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="103">
+      <c r="B5" s="94">
         <f>COUNTA(Confronto!B3:B270)</f>
         <v>268</v>
       </c>
@@ -68245,7 +68225,7 @@
       <c r="A6" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="105">
+      <c r="B6" s="96">
         <f>B5-B4</f>
         <v>94</v>
       </c>
@@ -68287,7 +68267,7 @@
       <c r="A7" t="s">
         <v>288</v>
       </c>
-      <c r="B7" s="106">
+      <c r="B7" s="97">
         <f>B4/B5</f>
         <v>0.64925373134328357</v>
       </c>
@@ -68325,28 +68305,28 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="103"/>
-      <c r="C8" s="102" t="s">
-        <v>293</v>
-      </c>
-      <c r="D8" s="100">
+      <c r="B8" s="94"/>
+      <c r="C8" s="93" t="s">
+        <v>291</v>
+      </c>
+      <c r="D8" s="92">
         <f>AVERAGE(C7:J7)</f>
         <v>0.70615671641791056</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="86" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" s="107" t="s">
-        <v>295</v>
+        <v>292</v>
+      </c>
+      <c r="B9" s="98" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="103"/>
+      <c r="B10" s="94"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="103"/>
+      <c r="B11" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>